<commit_message>
read excel and create json
</commit_message>
<xml_diff>
--- a/py-training/src/com230-excel/gym_classes_instructors_data.xlsx
+++ b/py-training/src/com230-excel/gym_classes_instructors_data.xlsx
@@ -15,7 +15,7 @@
     <sheet name="schedule" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">enrolments!$D$1:$D$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">enrolments!$D$1:$D$34</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -273,17 +273,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY/MM/DD\ HH:MM"/>
-    <numFmt numFmtId="166" formatCode="YYYY/MM/DD"/>
-    <numFmt numFmtId="167" formatCode="HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="YYYY/MM/DD"/>
+    <numFmt numFmtId="166" formatCode="HH:MM"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -343,7 +343,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -352,15 +352,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,10 +372,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -393,7 +385,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,15 +506,15 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -538,7 +530,7 @@
       <c r="D1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -556,7 +548,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>43831.6040393519</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,7 +565,7 @@
         <v>21</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>43832.6040393519</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,7 +582,7 @@
         <v>24</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>43833.6040393518</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,7 +599,7 @@
         <v>27</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>43834.6040393519</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -624,7 +616,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>43835.6040393519</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,7 +633,7 @@
         <v>33</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>43836.6040393519</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,7 +650,7 @@
         <v>36</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>43837.6040393518</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,7 +667,7 @@
         <v>39</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>43838.6040393519</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,7 +684,7 @@
         <v>42</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>43839.6040393519</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,13 +701,13 @@
         <v>45</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>43840.6040393519</v>
+        <v>43831</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -728,17 +720,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,7 +757,7 @@
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="1" t="n">
         <v>43836</v>
       </c>
     </row>
@@ -779,7 +771,7 @@
       <c r="C3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="1" t="n">
         <v>43837</v>
       </c>
     </row>
@@ -793,7 +785,7 @@
       <c r="C4" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="1" t="n">
         <v>43838</v>
       </c>
     </row>
@@ -807,10 +799,9 @@
       <c r="C5" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="1" t="n">
         <v>43839</v>
       </c>
-      <c r="E5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -822,7 +813,7 @@
       <c r="C6" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="1" t="n">
         <v>43840</v>
       </c>
     </row>
@@ -836,7 +827,7 @@
       <c r="C7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="1" t="n">
         <v>43836</v>
       </c>
     </row>
@@ -850,7 +841,7 @@
       <c r="C8" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="1" t="n">
         <v>43837</v>
       </c>
     </row>
@@ -864,7 +855,7 @@
       <c r="C9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="1" t="n">
         <v>43838</v>
       </c>
     </row>
@@ -878,7 +869,7 @@
       <c r="C10" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="1" t="n">
         <v>43837</v>
       </c>
     </row>
@@ -892,7 +883,7 @@
       <c r="C11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="1" t="n">
         <v>43836</v>
       </c>
     </row>
@@ -906,7 +897,7 @@
       <c r="C12" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="1" t="n">
         <v>43837</v>
       </c>
     </row>
@@ -920,7 +911,7 @@
       <c r="C13" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="1" t="n">
         <v>43838</v>
       </c>
     </row>
@@ -934,7 +925,7 @@
       <c r="C14" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D14" s="1" t="n">
         <v>43839</v>
       </c>
     </row>
@@ -948,7 +939,7 @@
       <c r="C15" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D15" s="3" t="n">
+      <c r="D15" s="1" t="n">
         <v>43840</v>
       </c>
     </row>
@@ -962,7 +953,7 @@
       <c r="C16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D16" s="1" t="n">
         <v>43836</v>
       </c>
     </row>
@@ -976,7 +967,7 @@
       <c r="C17" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D17" s="3" t="n">
+      <c r="D17" s="1" t="n">
         <v>43837</v>
       </c>
     </row>
@@ -990,7 +981,7 @@
       <c r="C18" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D18" s="3" t="n">
+      <c r="D18" s="1" t="n">
         <v>43838</v>
       </c>
     </row>
@@ -1004,7 +995,7 @@
       <c r="C19" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D19" s="3" t="n">
+      <c r="D19" s="1" t="n">
         <v>43839</v>
       </c>
     </row>
@@ -1018,7 +1009,7 @@
       <c r="C20" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="1" t="n">
         <v>43840</v>
       </c>
     </row>
@@ -1032,7 +1023,7 @@
       <c r="C21" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="1" t="n">
         <v>43840</v>
       </c>
     </row>
@@ -1046,7 +1037,7 @@
       <c r="C22" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="1" t="n">
         <v>43836</v>
       </c>
     </row>
@@ -1060,7 +1051,7 @@
       <c r="C23" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D23" s="3" t="n">
+      <c r="D23" s="1" t="n">
         <v>43837</v>
       </c>
     </row>
@@ -1074,7 +1065,7 @@
       <c r="C24" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D24" s="3" t="n">
+      <c r="D24" s="1" t="n">
         <v>43838</v>
       </c>
     </row>
@@ -1088,7 +1079,7 @@
       <c r="C25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="3" t="n">
+      <c r="D25" s="1" t="n">
         <v>43836</v>
       </c>
     </row>
@@ -1102,7 +1093,7 @@
       <c r="C26" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D26" s="3" t="n">
+      <c r="D26" s="1" t="n">
         <v>43837</v>
       </c>
     </row>
@@ -1116,7 +1107,7 @@
       <c r="C27" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D27" s="3" t="n">
+      <c r="D27" s="1" t="n">
         <v>43839</v>
       </c>
     </row>
@@ -1130,7 +1121,7 @@
       <c r="C28" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D28" s="3" t="n">
+      <c r="D28" s="1" t="n">
         <v>43836</v>
       </c>
     </row>
@@ -1144,7 +1135,7 @@
       <c r="C29" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D29" s="3" t="n">
+      <c r="D29" s="1" t="n">
         <v>43837</v>
       </c>
     </row>
@@ -1158,7 +1149,7 @@
       <c r="C30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D30" s="3" t="n">
+      <c r="D30" s="1" t="n">
         <v>43836</v>
       </c>
     </row>
@@ -1172,7 +1163,7 @@
       <c r="C31" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D31" s="3" t="n">
+      <c r="D31" s="1" t="n">
         <v>43837</v>
       </c>
     </row>
@@ -1186,7 +1177,7 @@
       <c r="C32" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D32" s="3" t="n">
+      <c r="D32" s="1" t="n">
         <v>43837</v>
       </c>
     </row>
@@ -1200,7 +1191,7 @@
       <c r="C33" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D33" s="3" t="n">
+      <c r="D33" s="1" t="n">
         <v>43839</v>
       </c>
     </row>
@@ -1214,20 +1205,18 @@
       <c r="C34" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D34" s="3" t="n">
+      <c r="D34" s="1" t="n">
         <v>43840</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D34"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1244,9 +1233,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1354,7 +1343,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1370,14 +1359,14 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,7 +1382,7 @@
       <c r="D1" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -1413,7 +1402,7 @@
       <c r="D2" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="3" t="n">
         <v>0.770833333333333</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -1433,7 +1422,7 @@
       <c r="D3" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="3" t="n">
         <v>0.6875</v>
       </c>
       <c r="F3" s="0" t="s">
@@ -1453,7 +1442,7 @@
       <c r="D4" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="3" t="n">
         <v>0.354166666666667</v>
       </c>
       <c r="F4" s="0" t="s">
@@ -1473,7 +1462,7 @@
       <c r="D5" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="3" t="n">
         <v>0.4375</v>
       </c>
       <c r="F5" s="0" t="s">
@@ -1493,7 +1482,7 @@
       <c r="D6" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="3" t="n">
         <v>0.729166666666667</v>
       </c>
       <c r="F6" s="0" t="s">
@@ -1513,7 +1502,7 @@
       <c r="D7" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="3" t="n">
         <v>0.770833333333333</v>
       </c>
       <c r="F7" s="0" t="s">
@@ -1533,7 +1522,7 @@
       <c r="D8" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="3" t="n">
         <v>0.8125</v>
       </c>
       <c r="F8" s="0" t="s">
@@ -1553,7 +1542,7 @@
       <c r="D9" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="E9" s="3" t="n">
         <v>0.770833333333333</v>
       </c>
       <c r="F9" s="0" t="s">
@@ -1573,7 +1562,7 @@
       <c r="D10" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="3" t="n">
         <v>0.770833333333333</v>
       </c>
       <c r="F10" s="0" t="s">
@@ -1593,7 +1582,7 @@
       <c r="D11" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E11" s="3" t="n">
         <v>0.770833333333333</v>
       </c>
       <c r="F11" s="0" t="s">
@@ -1603,7 +1592,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
access data for report
</commit_message>
<xml_diff>
--- a/py-training/src/com230-excel/gym_classes_instructors_data.xlsx
+++ b/py-training/src/com230-excel/gym_classes_instructors_data.xlsx
@@ -5,17 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="customers" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="enrolments" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="invoices" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="instructors" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="schedule" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">enrolments!$D$1:$D$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">invoices!$D$1:$D$34</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
   <si>
     <t xml:space="preserve">class_id</t>
   </si>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">personal training</t>
   </si>
   <si>
-    <t xml:space="preserve">customer_Id</t>
+    <t xml:space="preserve">customer_id</t>
   </si>
   <si>
     <t xml:space="preserve">first_name</t>
@@ -167,16 +167,16 @@
     <t xml:space="preserve">britten.jen@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">enrolment_Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schedule_Id</t>
+    <t xml:space="preserve">invoice_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schedule_id</t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">instructor_Id</t>
+    <t xml:space="preserve">instructor_id</t>
   </si>
   <si>
     <t xml:space="preserve">phone</t>
@@ -234,9 +234,6 @@
   </si>
   <si>
     <t xml:space="preserve">403-987-3682</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class_Id</t>
   </si>
   <si>
     <t xml:space="preserve">schedule_day</t>
@@ -505,7 +502,7 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -722,8 +719,8 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1228,7 +1225,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1359,7 +1356,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1374,19 +1371,19 @@
         <v>47</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>49</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1400,13 +1397,13 @@
         <v>3</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>0.770833333333333</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1420,13 +1417,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>0.6875</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,13 +1437,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>0.354166666666667</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1460,13 +1457,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>0.4375</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1480,13 +1477,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>0.729166666666667</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,13 +1497,13 @@
         <v>5</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>0.770833333333333</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1520,13 +1517,13 @@
         <v>4</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>0.8125</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,13 +1537,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>0.770833333333333</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1560,13 +1557,13 @@
         <v>2</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>0.770833333333333</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,13 +1577,13 @@
         <v>5</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>0.770833333333333</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
invoice report created based on customer_id input
</commit_message>
<xml_diff>
--- a/py-training/src/com230-excel/gym_classes_instructors_data.xlsx
+++ b/py-training/src/com230-excel/gym_classes_instructors_data.xlsx
@@ -65,10 +65,10 @@
     <t xml:space="preserve">customer_id</t>
   </si>
   <si>
-    <t xml:space="preserve">first_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last_name</t>
+    <t xml:space="preserve">f_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l_name</t>
   </si>
   <si>
     <t xml:space="preserve">email</t>
@@ -381,9 +381,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -503,15 +500,13 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,9 +720,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1225,14 +1218,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,9 +1352,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="12.9591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>